<commit_message>
Exported sample size flowchart for report
</commit_message>
<xml_diff>
--- a/proposal/mango_tango_pramoda_v2.xlsx
+++ b/proposal/mango_tango_pramoda_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sachijay_student_ubc_ca/Documents/courses/spph_604_application_of_advanced_epidemiological_methods/spph604_final_project/proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="634" documentId="11_9E716DB01F0E853FD979700CD91846EF7618449E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5B59B0F-6C45-4B93-99E5-C0CFB34E8D76}"/>
+  <xr:revisionPtr revIDLastSave="639" documentId="11_9E716DB01F0E853FD979700CD91846EF7618449E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0138BAF5-2EED-4E93-8C57-4F72C0CAD293}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="18700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5115" yWindow="3450" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Research Question" sheetId="2" r:id="rId1"/>
@@ -969,118 +969,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBA834AE-5DF0-4F64-99AE-55D8412C6134}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="2"/>
-          <a:endCxn id="4" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3019425" y="1552575"/>
-          <a:ext cx="9525" cy="657225"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B588A110-39FD-4221-A9BA-64A4D9A6EE81}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="4" idx="2"/>
-          <a:endCxn id="10" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3009900" y="3352800"/>
-          <a:ext cx="9525" cy="657225"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -1094,10 +982,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="24" name="Group 23">
+        <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3CE0486-8CCB-EFB7-B84E-C6BED11265F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73577340-C5FC-F6A4-5053-830EB6614B1B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1105,214 +993,38 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1786591" y="402104"/>
-          <a:ext cx="6127190" cy="8173758"/>
-          <a:chOff x="866775" y="447675"/>
-          <a:chExt cx="5838825" cy="8334375"/>
+          <a:off x="1704415" y="409575"/>
+          <a:ext cx="5798484" cy="8334375"/>
+          <a:chOff x="1704415" y="409575"/>
+          <a:chExt cx="5798484" cy="8334375"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 2">
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AC29976-5916-5F9E-4A5E-014BED8D6577}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="885825" y="447675"/>
-            <a:ext cx="2590800" cy="1143000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>Total number of 2015-2016 and 2017-2020 respondents</a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="en-CA" sz="1400"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>n = 25,531</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Rectangle 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65304C6B-BCF8-4593-8C74-1D6B9B4FB9D5}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="876300" y="2247900"/>
-            <a:ext cx="2590800" cy="1143000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>Asthma patients</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>n</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-              <a:t> = 3,765 (14.7%)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CA" sz="1400"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Rectangle 4">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{465E79BD-8320-4737-B4C4-3E53A89A08C8}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4114800" y="1343025"/>
-            <a:ext cx="2590800" cy="1143000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>Non</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-              <a:t> asthma patients</a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="en-CA" sz="1400"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>n = 21,766</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BA3BB66-BDF1-C2E8-C008-3510A2527CC3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBA834AE-5DF0-4F64-99AE-55D8412C6134}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
-            <a:endCxn id="5" idx="1"/>
+            <a:stCxn id="3" idx="2"/>
+            <a:endCxn id="4" idx="0"/>
           </xdr:cNvCxnSpPr>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2181225" y="1914525"/>
-            <a:ext cx="1933575" cy="0"/>
+          <a:xfrm flipH="1">
+            <a:off x="2999254" y="1552575"/>
+            <a:ext cx="9525" cy="657225"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
           </a:prstGeom>
           <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
             <a:tailEnd type="triangle"/>
           </a:ln>
         </xdr:spPr>
@@ -1331,152 +1043,32 @@
           </a:fontRef>
         </xdr:style>
       </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="Rectangle 9">
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E08CD646-9DF5-46F3-AEF3-9BE2508C4D92}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="866775" y="4048125"/>
-            <a:ext cx="2590800" cy="1143000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>20</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-              <a:t> years or older</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CA" sz="1400"/>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>n</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-              <a:t> = 2,284 (8.9%)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CA" sz="1400"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="Rectangle 13">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B82976E-44A9-4C24-8A50-A98D3FF7B5D9}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4114800" y="3133725"/>
-            <a:ext cx="2590800" cy="1143000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>Less than 20 years old</a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="en-CA" sz="1400"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>n = 1,481</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55B6E583-F8D1-41DE-9557-A3042782EB1D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B588A110-39FD-4221-A9BA-64A4D9A6EE81}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
-            <a:endCxn id="14" idx="1"/>
+            <a:stCxn id="4" idx="2"/>
+            <a:endCxn id="10" idx="0"/>
           </xdr:cNvCxnSpPr>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2181225" y="3705225"/>
-            <a:ext cx="1933575" cy="0"/>
+          <a:xfrm flipH="1">
+            <a:off x="2989729" y="3352800"/>
+            <a:ext cx="9525" cy="657225"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
           </a:prstGeom>
           <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
             <a:tailEnd type="triangle"/>
           </a:ln>
         </xdr:spPr>
@@ -1495,412 +1087,870 @@
           </a:fontRef>
         </xdr:style>
       </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="16" name="Rectangle 15">
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="24" name="Group 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94B8059B-CCA7-44F4-8C53-05EEE402A702}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3CE0486-8CCB-EFB7-B84E-C6BED11265F3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="866775" y="5848350"/>
-            <a:ext cx="2590800" cy="1143000"/>
+            <a:off x="1704415" y="409575"/>
+            <a:ext cx="5798484" cy="8334375"/>
+            <a:chOff x="866775" y="447675"/>
+            <a:chExt cx="5838825" cy="8334375"/>
           </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>Non-missing values for insurance status</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>n</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-              <a:t> = 2,275 (8.9%)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CA" sz="1400"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C8C0011-B6F5-44CC-8816-D284A76A02F9}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:endCxn id="16" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="2162175" y="5191125"/>
-            <a:ext cx="9525" cy="657225"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="18" name="Rectangle 17">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E21B67-A5BD-49F9-8DA1-CB494176803C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4114800" y="4953000"/>
-            <a:ext cx="2590800" cy="1143000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>Missing values for</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-              <a:t> insurance</a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="en-CA" sz="1400"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>n = 9</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34C1F8C4-83FB-478E-9F26-DEC0475952BD}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:endCxn id="18" idx="1"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2181225" y="5524500"/>
-            <a:ext cx="1933575" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="20" name="Rectangle 19">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F7E3AF0-A90C-438C-B878-AC39CE7DED0E}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="866775" y="7639050"/>
-            <a:ext cx="2590800" cy="1143000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>Non-missing values for COPD, emphysema, or chronic bronchitis</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>n</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-              <a:t> = 2,264 (8.9%)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CA" sz="1400"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC732DE4-28EC-4A82-BBE8-64486EF79E20}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:endCxn id="20" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="2162175" y="6981825"/>
-            <a:ext cx="9525" cy="657225"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="22" name="Rectangle 21">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80C6B6BA-92E8-4B94-9198-CBD7829A402A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4105275" y="6734175"/>
-            <a:ext cx="2590800" cy="1143000"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:headEnd type="none" w="med" len="med"/>
-            <a:tailEnd type="none" w="med" len="med"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>Missing values for</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-              <a:t> COPD, emphysema, or chronic bronchitis</a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="en-CA" sz="1400"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1400"/>
-              <a:t>n = 9</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{536029C3-E1B4-4FD2-90FE-41347BA7F93B}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:endCxn id="22" idx="1"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2171700" y="7305675"/>
-            <a:ext cx="1933575" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="Rectangle 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AC29976-5916-5F9E-4A5E-014BED8D6577}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="885825" y="447675"/>
+              <a:ext cx="2590800" cy="1143000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>Total number of 2015-2016 and 2017-2020 respondents</a:t>
+              </a:r>
+              <a:br>
+                <a:rPr lang="en-CA" sz="1400"/>
+              </a:br>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>n = 25,531</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="Rectangle 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65304C6B-BCF8-4593-8C74-1D6B9B4FB9D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="876300" y="2247900"/>
+              <a:ext cx="2590800" cy="1143000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>Asthma patients</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>n</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400" baseline="0"/>
+                <a:t> = 3,765 (14.7%)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-CA" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="Rectangle 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{465E79BD-8320-4737-B4C4-3E53A89A08C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4114800" y="1343025"/>
+              <a:ext cx="2590800" cy="1143000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>Non</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400" baseline="0"/>
+                <a:t> asthma patients</a:t>
+              </a:r>
+              <a:br>
+                <a:rPr lang="en-CA" sz="1400"/>
+              </a:br>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>n = 21,766</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BA3BB66-BDF1-C2E8-C008-3510A2527CC3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="5" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2181225" y="1914525"/>
+              <a:ext cx="1933575" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="Rectangle 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E08CD646-9DF5-46F3-AEF3-9BE2508C4D92}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="866775" y="4048125"/>
+              <a:ext cx="2590800" cy="1143000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>20</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400" baseline="0"/>
+                <a:t> years or older</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-CA" sz="1400"/>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>n</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400" baseline="0"/>
+                <a:t> = 2,284 (8.9%)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-CA" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="Rectangle 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B82976E-44A9-4C24-8A50-A98D3FF7B5D9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4114800" y="3133725"/>
+              <a:ext cx="2590800" cy="1143000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>Less than 20 years old</a:t>
+              </a:r>
+              <a:br>
+                <a:rPr lang="en-CA" sz="1400"/>
+              </a:br>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>n = 1,481</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55B6E583-F8D1-41DE-9557-A3042782EB1D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="14" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2181225" y="3705225"/>
+              <a:ext cx="1933575" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="Rectangle 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94B8059B-CCA7-44F4-8C53-05EEE402A702}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="866775" y="5848350"/>
+              <a:ext cx="2590800" cy="1143000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>Non-missing values for insurance status</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>n</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400" baseline="0"/>
+                <a:t> = 2,275 (8.9%)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-CA" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C8C0011-B6F5-44CC-8816-D284A76A02F9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="16" idx="0"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="2162175" y="5191125"/>
+              <a:ext cx="9525" cy="657225"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="18" name="Rectangle 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E21B67-A5BD-49F9-8DA1-CB494176803C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4114800" y="4953000"/>
+              <a:ext cx="2590800" cy="1143000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>Missing values for</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400" baseline="0"/>
+                <a:t> insurance</a:t>
+              </a:r>
+              <a:br>
+                <a:rPr lang="en-CA" sz="1400"/>
+              </a:br>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>n = 9</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34C1F8C4-83FB-478E-9F26-DEC0475952BD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="18" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2181225" y="5524500"/>
+              <a:ext cx="1933575" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="20" name="Rectangle 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F7E3AF0-A90C-438C-B878-AC39CE7DED0E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="866775" y="7639050"/>
+              <a:ext cx="2590800" cy="1143000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>Non-missing values for COPD, emphysema, or chronic bronchitis</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>n</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400" baseline="0"/>
+                <a:t> = 2,264 (8.9%)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-CA" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC732DE4-28EC-4A82-BBE8-64486EF79E20}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="20" idx="0"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipH="1">
+              <a:off x="2162175" y="6981825"/>
+              <a:ext cx="9525" cy="657225"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="22" name="Rectangle 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80C6B6BA-92E8-4B94-9198-CBD7829A402A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4105275" y="6734175"/>
+              <a:ext cx="2590800" cy="1143000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>Missing values for</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400" baseline="0"/>
+                <a:t> COPD, emphysema, or chronic bronchitis</a:t>
+              </a:r>
+              <a:br>
+                <a:rPr lang="en-CA" sz="1400"/>
+              </a:br>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1400"/>
+                <a:t>n = 9</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{536029C3-E1B4-4FD2-90FE-41347BA7F93B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvCxnSpPr>
+              <a:endCxn id="22" idx="1"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2171700" y="7305675"/>
+              <a:ext cx="1933575" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent2"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent2"/>
+            </a:fillRef>
+            <a:effectRef idx="1">
+              <a:schemeClr val="accent2"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+      </xdr:grpSp>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -2249,19 +2299,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="6"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="27" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44.453125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="62.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2271,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -2285,7 +2335,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
@@ -2299,7 +2349,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -2313,7 +2363,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -2327,7 +2377,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
@@ -2339,18 +2389,18 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
     </row>
-    <row r="9" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
         <v>13</v>
@@ -2359,7 +2409,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="16" t="s">
         <v>14</v>
@@ -2368,18 +2418,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
     </row>
-    <row r="13" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="19" t="s">
         <v>16</v>
@@ -2389,7 +2439,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
@@ -2400,7 +2450,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="13" t="s">
         <v>19</v>
@@ -2409,7 +2459,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="16" t="s">
         <v>20</v>
@@ -2418,7 +2468,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="10" t="s">
         <v>21</v>
@@ -2427,32 +2477,32 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="13"/>
       <c r="C20" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="13"/>
       <c r="C21" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="24"/>
       <c r="C22" s="17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
     </row>
-    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="25" t="s">
         <v>22</v>
@@ -2464,7 +2514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="7" t="s">
         <v>53</v>
@@ -2476,7 +2526,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="7" t="s">
         <v>50</v>
@@ -2488,7 +2538,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="7" t="s">
         <v>54</v>
@@ -2500,7 +2550,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="7" t="s">
         <v>172</v>
@@ -2512,7 +2562,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="7" t="s">
         <v>169</v>
@@ -2524,7 +2574,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="7" t="s">
         <v>170</v>
@@ -2536,7 +2586,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
       <c r="B31" s="7" t="s">
         <v>162</v>
@@ -2548,19 +2598,19 @@
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="18"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="26"/>
       <c r="B33" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="6" t="s">
         <v>85</v>
@@ -2572,7 +2622,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="26"/>
       <c r="B35" s="6" t="s">
         <v>44</v>
@@ -2584,19 +2634,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
       <c r="B36" s="18"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="26"/>
       <c r="B37" s="13" t="s">
         <v>65</v>
       </c>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="7" t="s">
         <v>63</v>
@@ -2605,7 +2655,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="26"/>
       <c r="B39" s="7" t="s">
         <v>47</v>
@@ -2614,13 +2664,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="27"/>
       <c r="C40" s="24"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>25</v>
       </c>
@@ -2629,40 +2679,40 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
       <c r="B43" s="7"/>
       <c r="C43" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
       <c r="B44" s="7"/>
       <c r="C44" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="7"/>
       <c r="C45" s="31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="32"/>
       <c r="B46" s="24"/>
       <c r="C46" s="17"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B48" s="33"/>
       <c r="C48" s="11"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="32"/>
       <c r="B49" s="24"/>
       <c r="C49" s="17" t="s">
@@ -2680,10 +2730,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2694,26 +2744,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G102" sqref="G102"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.54296875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="33.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="6" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>28</v>
       </c>
@@ -2745,7 +2795,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="42"/>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
@@ -2757,7 +2807,7 @@
       <c r="I3" s="43"/>
       <c r="J3" s="42"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>175</v>
       </c>
@@ -2783,12 +2833,12 @@
       <c r="I4" s="44"/>
       <c r="J4" s="28"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7"/>
       <c r="F5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>176</v>
       </c>
@@ -2812,7 +2862,7 @@
       </c>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
         <v>98</v>
       </c>
@@ -2823,12 +2873,12 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="F8" s="7"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>177</v>
       </c>
@@ -2857,7 +2907,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="34" t="s">
         <v>98</v>
@@ -2874,7 +2924,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="36"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -2884,7 +2934,7 @@
       <c r="G11" s="35"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>178</v>
       </c>
@@ -2916,7 +2966,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="F13" s="7"/>
@@ -2930,7 +2980,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="F14" s="7"/>
@@ -2941,13 +2991,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="F15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>179</v>
       </c>
@@ -2976,7 +3026,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="F17" s="7"/>
@@ -2988,14 +3038,14 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="F18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>180</v>
       </c>
@@ -3024,7 +3074,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="F20" s="7"/>
@@ -3035,7 +3085,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="F21" s="7"/>
@@ -3046,7 +3096,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="F22" s="7"/>
@@ -3057,7 +3107,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="F23" s="7"/>
@@ -3065,13 +3115,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="F24" s="7"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>181</v>
       </c>
@@ -3103,7 +3153,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="F26" s="7"/>
@@ -3117,7 +3167,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="F27" s="7"/>
@@ -3131,7 +3181,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="F28" s="7"/>
@@ -3145,7 +3195,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="F29" s="7"/>
@@ -3156,7 +3206,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>108</v>
       </c>
@@ -3185,7 +3235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="F31" s="7"/>
@@ -3199,7 +3249,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="F32" s="7"/>
@@ -3213,7 +3263,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="F33" s="7"/>
@@ -3227,7 +3277,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="F34" s="7"/>
@@ -3238,7 +3288,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>108</v>
       </c>
@@ -3267,7 +3317,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="F36" s="7"/>
@@ -3281,7 +3331,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="F37" s="7"/>
@@ -3295,7 +3345,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="F38" s="7"/>
@@ -3309,7 +3359,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="F39" s="7"/>
@@ -3320,7 +3370,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>118</v>
       </c>
@@ -3349,7 +3399,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="F41" s="7"/>
@@ -3363,7 +3413,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="F42" s="7"/>
@@ -3377,7 +3427,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="F43" s="7"/>
@@ -3391,7 +3441,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="F44" s="7"/>
@@ -3402,14 +3452,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="F45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>182</v>
       </c>
@@ -3441,7 +3491,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="F47" s="7"/>
@@ -3455,7 +3505,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="F48" s="7"/>
@@ -3469,7 +3519,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="F49" s="7"/>
@@ -3483,7 +3533,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="F50" s="7"/>
@@ -3494,13 +3544,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="F51" s="7"/>
       <c r="I51" s="7"/>
     </row>
-    <row r="52" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>183</v>
       </c>
@@ -3532,7 +3582,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="F53" s="7"/>
@@ -3546,7 +3596,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="F54" s="7"/>
@@ -3560,7 +3610,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="F55" s="7"/>
@@ -3574,7 +3624,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="F56" s="7"/>
@@ -3585,7 +3635,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="F57" s="7"/>
@@ -3593,7 +3643,7 @@
       <c r="H57" s="39"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>184</v>
       </c>
@@ -3625,7 +3675,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="F59" s="7"/>
@@ -3639,7 +3689,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="F60" s="7"/>
@@ -3653,7 +3703,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="F61" s="7"/>
@@ -3664,7 +3714,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="F62" s="7"/>
@@ -3678,14 +3728,14 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="F63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>185</v>
       </c>
@@ -3717,7 +3767,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C65" s="7"/>
       <c r="F65" s="7"/>
       <c r="H65" s="35">
@@ -3730,7 +3780,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="F66" s="7"/>
@@ -3744,7 +3794,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="F67" s="7"/>
@@ -3758,7 +3808,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="F68" s="7"/>
@@ -3772,7 +3822,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="F69" s="7"/>
@@ -3786,7 +3836,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="F70" s="7"/>
@@ -3800,7 +3850,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="F71" s="7"/>
@@ -3814,7 +3864,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="F72" s="7"/>
@@ -3825,7 +3875,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" s="7" t="s">
         <v>130</v>
       </c>
@@ -3844,7 +3894,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="F74" s="7"/>
@@ -3858,7 +3908,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="F75" s="7"/>
@@ -3872,7 +3922,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="F76" s="7"/>
@@ -3886,7 +3936,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="F77" s="7"/>
@@ -3900,7 +3950,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="F78" s="7"/>
@@ -3914,7 +3964,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="F79" s="7"/>
@@ -3928,7 +3978,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="F80" s="7"/>
@@ -3939,13 +3989,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="F81" s="7"/>
       <c r="I81" s="7"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>186</v>
       </c>
@@ -3977,7 +4027,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="F83" s="7"/>
@@ -3991,7 +4041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="F84" s="7"/>
@@ -4005,7 +4055,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="F85" s="7"/>
@@ -4019,7 +4069,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="F86" s="7"/>
@@ -4030,13 +4080,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="F87" s="7"/>
       <c r="I87" s="7"/>
     </row>
-    <row r="88" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>187</v>
       </c>
@@ -4068,7 +4118,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="F89" s="7"/>
@@ -4082,7 +4132,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="F90" s="7"/>
@@ -4096,7 +4146,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="F91" s="7"/>
@@ -4110,7 +4160,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I92" s="7" t="s">
         <v>106</v>
       </c>
@@ -4118,7 +4168,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>188</v>
       </c>
@@ -4144,7 +4194,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H95" s="35">
         <v>777</v>
       </c>
@@ -4155,7 +4205,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H96" s="35">
         <v>999</v>
       </c>
@@ -4166,7 +4216,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I97" s="7" t="s">
         <v>106</v>
       </c>
@@ -4174,7 +4224,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>189</v>
       </c>
@@ -4206,7 +4256,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H100" s="35">
         <v>2</v>
       </c>
@@ -4217,7 +4267,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H101" s="35">
         <v>3</v>
       </c>
@@ -4228,7 +4278,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H102" s="35">
         <v>7</v>
       </c>
@@ -4239,7 +4289,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H103" s="35">
         <v>9</v>
       </c>
@@ -4250,7 +4300,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I104" s="7" t="s">
         <v>106</v>
       </c>
@@ -4280,13 +4330,13 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.7265625" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -4306,7 +4356,7 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4319,6 +4369,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100057B93E3E20B764A90AAF7BC46CF1D0D" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7f00a5ab9c88f7c55bc2fcf8324c26ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f04874dd-c440-4111-a52d-1fd467c9d483" xmlns:ns3="c2c2b2a6-1b83-46a5-b1dc-df5f446969f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4a0d2651c7d1bf3775b1c735c193b7e8" ns2:_="" ns3:_="">
     <xsd:import namespace="f04874dd-c440-4111-a52d-1fd467c9d483"/>
@@ -4489,15 +4548,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B93AC53-561C-494C-B1B9-280B080339A5}">
   <ds:schemaRefs>
@@ -4508,6 +4558,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B6F3028-2F04-400C-A5AD-14DDA34A20D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A604F10F-5481-4CA9-B757-82F0554D3F02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4524,12 +4582,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B6F3028-2F04-400C-A5AD-14DDA34A20D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added older than 80 exclusion
</commit_message>
<xml_diff>
--- a/proposal/mango_tango_pramoda_v2.xlsx
+++ b/proposal/mango_tango_pramoda_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sachijay_student_ubc_ca/Documents/courses/spph_604_application_of_advanced_epidemiological_methods/spph604_final_project/proposal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="639" documentId="11_9E716DB01F0E853FD979700CD91846EF7618449E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0138BAF5-2EED-4E93-8C57-4F72C0CAD293}"/>
+  <xr:revisionPtr revIDLastSave="655" documentId="11_9E716DB01F0E853FD979700CD91846EF7618449E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AD1B9A5-241E-4591-AB72-0E0EF5A9295A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5115" yWindow="3450" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33915" yWindow="3450" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Research Question" sheetId="2" r:id="rId1"/>
@@ -1390,13 +1390,8 @@
               <a:pPr algn="ctr"/>
               <a:r>
                 <a:rPr lang="en-CA" sz="1400"/>
-                <a:t>20</a:t>
+                <a:t>20 - 80 years old</a:t>
               </a:r>
-              <a:r>
-                <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-                <a:t> years or older</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-CA" sz="1400"/>
             </a:p>
             <a:p>
               <a:pPr algn="ctr"/>
@@ -1406,7 +1401,7 @@
               </a:r>
               <a:r>
                 <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-                <a:t> = 2,284 (8.9%)</a:t>
+                <a:t> = 2,172 (8.5%)</a:t>
               </a:r>
               <a:endParaRPr lang="en-CA" sz="1400"/>
             </a:p>
@@ -1461,14 +1456,14 @@
               <a:pPr algn="ctr"/>
               <a:r>
                 <a:rPr lang="en-CA" sz="1400"/>
-                <a:t>Less than 20 years old</a:t>
+                <a:t>Less than 20 years old or older than 80 years</a:t>
               </a:r>
               <a:br>
                 <a:rPr lang="en-CA" sz="1400"/>
               </a:br>
               <a:r>
                 <a:rPr lang="en-CA" sz="1400"/>
-                <a:t>n = 1,481</a:t>
+                <a:t>n = 1,593</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -1576,7 +1571,7 @@
               </a:r>
               <a:r>
                 <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-                <a:t> = 2,275 (8.9%)</a:t>
+                <a:t> = 2,164 (8.5%)</a:t>
               </a:r>
               <a:endParaRPr lang="en-CA" sz="1400"/>
             </a:p>
@@ -1685,7 +1680,7 @@
               </a:br>
               <a:r>
                 <a:rPr lang="en-CA" sz="1400"/>
-                <a:t>n = 9</a:t>
+                <a:t>n = 8</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -1793,7 +1788,7 @@
               </a:r>
               <a:r>
                 <a:rPr lang="en-CA" sz="1400" baseline="0"/>
-                <a:t> = 2,264 (8.9%)</a:t>
+                <a:t> = 2,154 (8.4%)</a:t>
               </a:r>
               <a:endParaRPr lang="en-CA" sz="1400"/>
             </a:p>
@@ -1902,7 +1897,7 @@
               </a:br>
               <a:r>
                 <a:rPr lang="en-CA" sz="1400"/>
-                <a:t>n = 9</a:t>
+                <a:t>n = 10</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -2299,7 +2294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B26" sqref="B26:B31"/>
     </sheetView>
   </sheetViews>
@@ -2729,8 +2724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4FF855-805C-49CB-9D63-C7E8A461572B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4363,18 +4358,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4549,18 +4544,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B93AC53-561C-494C-B1B9-280B080339A5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B6F3028-2F04-400C-A5AD-14DDA34A20D7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B6F3028-2F04-400C-A5AD-14DDA34A20D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B93AC53-561C-494C-B1B9-280B080339A5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>